<commit_message>
cd: update sch/sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/DRC/cd_sch_sth_baseline_1_school_202202.xlsx
+++ b/SCH-STH/Impact assessments/DRC/cd_sch_sth_baseline_1_school_202202.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12300" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -126,6 +126,30 @@
     <t>aire_sante = ${w_aire_sante}</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>w_ecole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Nom de l’école </t>
+  </si>
+  <si>
+    <t>w_code_ecole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. Code de l’école </t>
+  </si>
+  <si>
+    <t>Code à trois chiffre. Ex : 001</t>
+  </si>
+  <si>
+    <t>regex(.,'^[0-9]{3}$')</t>
+  </si>
+  <si>
+    <t>Le code doit être un nombre à deux chiffres</t>
+  </si>
+  <si>
     <t>geopoint</t>
   </si>
   <si>
@@ -138,30 +162,6 @@
     <t>Capturer les coordonnées GPS</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>w_ecole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8. Nom de l’école </t>
-  </si>
-  <si>
-    <t>w_code_ecole</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9. Code de l’école </t>
-  </si>
-  <si>
-    <t>Code à trois chiffre. Ex : 001</t>
-  </si>
-  <si>
-    <t>regex(.,'^[0-9]{3}$')</t>
-  </si>
-  <si>
-    <t>Le code doit être un nombre à deux chiffres</t>
-  </si>
-  <si>
     <t>w_chef_etbl</t>
   </si>
   <si>
@@ -720,10 +720,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>1. SCH/STH - Site</t>
-  </si>
-  <si>
-    <t>cd_sch_sth_baseline_1_school_202202</t>
+    <t>1. SCH/STH - Site V2</t>
+  </si>
+  <si>
+    <t>cd_sch_sth_baseline_1_school_202202_v2</t>
   </si>
   <si>
     <t>French</t>
@@ -735,9 +735,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -764,31 +764,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -796,14 +774,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -818,9 +788,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -833,7 +827,51 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -854,46 +892,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -907,9 +907,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -930,7 +930,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -942,13 +942,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -960,133 +1080,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1104,13 +1098,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1178,11 +1178,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1207,6 +1213,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1221,166 +1236,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1770,12 +1770,12 @@
   <sheetPr/>
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="$A5:$XFD5 $A7:$XFD7 $A12:$XFD12"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1997,76 +1997,76 @@
       <c r="C9" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>39</v>
-      </c>
+      <c r="D9" s="19"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="19"/>
       <c r="H9" s="16"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" s="3" customFormat="1" spans="1:12">
-      <c r="A10" s="12"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
+    <row r="10" s="3" customFormat="1" ht="28.5" spans="1:12">
+      <c r="A10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="19"/>
+      <c r="F10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>43</v>
+      </c>
       <c r="H10" s="16"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="J10" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="K10" s="8"/>
       <c r="L10" s="7"/>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:12">
-      <c r="A11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="A11" s="12"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="19"/>
       <c r="H11" s="16"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" s="3" customFormat="1" ht="28.5" spans="1:12">
+    <row r="12" s="3" customFormat="1" spans="1:12">
       <c r="A12" s="12" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>47</v>
-      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="16"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8" t="s">
@@ -2077,7 +2077,7 @@
     </row>
     <row r="13" s="3" customFormat="1" spans="1:12">
       <c r="A13" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>48</v>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="14" s="3" customFormat="1" spans="1:12">
       <c r="A14" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>50</v>
@@ -4520,8 +4520,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>

</xml_diff>